<commit_message>
GroupID uint8_t로 변경, WorldID, ServerID int16_t로 변경
</commit_message>
<xml_diff>
--- a/Document/Data/Config/ServerConfig.xlsx
+++ b/Document/Data/Config/ServerConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newmr\Desktop\Study\Core\Document\Data\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HavePoop\Desktop\Study\Core\Document\Data\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933181DF-72B8-4E47-AEEE-714F61A7D27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2D284C-C356-4E17-BE36-0824D1137A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="4095" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ServerConfig" sheetId="2" r:id="rId1"/>
@@ -57,11 +57,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int16_t</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -444,7 +444,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -464,13 +464,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -489,10 +489,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>